<commit_message>
cambio del vs de los pueblos originario
</commit_message>
<xml_diff>
--- a/fhir/ig/tei/CodeSystem-PueblosOriginariosCS.xlsx
+++ b/fhir/ig/tei/CodeSystem-PueblosOriginariosCS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-10-18T10:47:09-03:00</t>
+    <t>2024-02-20T17:14:58-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -189,13 +189,10 @@
     <t>Yagan</t>
   </si>
   <si>
+    <t>Chango</t>
+  </si>
+  <si>
     <t>10</t>
-  </si>
-  <si>
-    <t>Chango</t>
-  </si>
-  <si>
-    <t>96</t>
   </si>
   <si>
     <t>Otro (Especificar)</t>
@@ -644,10 +641,10 @@
         <v>39</v>
       </c>
       <c r="B11" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s" s="2">
         <v>58</v>
-      </c>
-      <c r="C11" t="s" s="2">
-        <v>59</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -656,10 +653,10 @@
         <v>39</v>
       </c>
       <c r="B12" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s" s="2">
         <v>60</v>
-      </c>
-      <c r="C12" t="s" s="2">
-        <v>61</v>
       </c>
       <c r="D12" s="2"/>
     </row>

</xml_diff>